<commit_message>
Generate PDF plots to check conc over time linearity. Flux calculation script generally good to go.
</commit_message>
<xml_diff>
--- a/Field_Data/Field_Data.xlsx
+++ b/Field_Data/Field_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11265"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11268"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -424,21 +424,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:C40"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J86" sqref="J86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +470,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -478,7 +478,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -486,7 +486,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -494,7 +494,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -502,7 +502,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -510,7 +510,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -518,7 +518,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -526,7 +526,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -534,7 +534,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -542,7 +542,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -550,7 +550,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -558,7 +558,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -566,7 +566,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -574,7 +574,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -582,7 +582,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -590,7 +590,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -598,7 +598,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -606,7 +606,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -614,7 +614,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -622,7 +622,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -630,7 +630,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -638,7 +638,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -646,7 +646,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -654,7 +654,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -662,7 +662,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -670,7 +670,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -678,7 +678,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -686,7 +686,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -694,7 +694,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -702,7 +702,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -710,7 +710,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -733,7 +733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -756,7 +756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -779,7 +779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -802,7 +802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -825,7 +825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -851,7 +851,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -883,7 +883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -906,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -938,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -961,7 +961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -984,7 +984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>20</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>21</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>9</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>17</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>18</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>19</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>20</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>21</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>9</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>11</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>12</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>13</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>45849</v>
       </c>
       <c r="C85" s="1">
-        <v>0.422222222222222</v>
+        <v>0.42291666666666666</v>
       </c>
       <c r="D85">
         <v>28.9</v>
@@ -2093,10 +2093,10 @@
         <v>2</v>
       </c>
       <c r="J85">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>17</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>18</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>19</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>20</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>21</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>7</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>9</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>12</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>13</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>15</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>17</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>18</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>19</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>20</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>21</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>7</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>8</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>9</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>10</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>11</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>12</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>13</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>14</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>15</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>16</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>17</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>19</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>20</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>21</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>7</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>8</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>9</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>10</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>11</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>12</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>13</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>14</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>15</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>16</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>17</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>18</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>19</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>20</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>45873</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>21</v>
       </c>

</xml_diff>